<commit_message>
Added 3 telehpne no. in branch and set mall and city selection in branch section > Add/Edit Store
</commit_message>
<xml_diff>
--- a/media/LocationsExcels/location.xlsx
+++ b/media/LocationsExcels/location.xlsx
@@ -11,12 +11,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>branch_name</t>
   </si>
   <si>
     <t>telephone_number</t>
+  </si>
+  <si>
+    <t>telephone_number_2</t>
+  </si>
+  <si>
+    <t>telephone_number_3</t>
   </si>
   <si>
     <t>email</t>
@@ -32,7 +38,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -42,13 +48,23 @@
       <color rgb="FF000000"/>
     </font>
     <font/>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -57,7 +73,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -65,10 +81,13 @@
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -99,16 +118,21 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>